<commit_message>
Auto-evalutation de l'avancement du projet
</commit_message>
<xml_diff>
--- a/evaluation/evaluation.xlsx
+++ b/evaluation/evaluation.xlsx
@@ -1,15 +1,18 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="23812"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="240" windowWidth="25360" windowHeight="16500" tabRatio="500"/>
+    <workbookView xWindow="240" yWindow="240" windowWidth="20730" windowHeight="11760" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="140000" concurrentCalc="0"/>
+  <definedNames>
+    <definedName name="LOCAL_MYSQL_DATE_FORMAT" hidden="1">REPT(LOCAL_YEAR_FORMAT,4)&amp;LOCAL_DATE_SEPARATOR&amp;REPT(LOCAL_MONTH_FORMAT,2)&amp;LOCAL_DATE_SEPARATOR&amp;REPT(LOCAL_DAY_FORMAT,2)&amp;" "&amp;REPT(LOCAL_HOUR_FORMAT,2)&amp;LOCAL_TIME_SEPARATOR&amp;REPT(LOCAL_MINUTE_FORMAT,2)&amp;LOCAL_TIME_SEPARATOR&amp;REPT(LOCAL_SECOND_FORMAT,2)</definedName>
+  </definedNames>
+  <calcPr calcId="145621" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -19,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="53">
   <si>
     <t>LIVRABLES</t>
   </si>
@@ -160,6 +163,24 @@
   </si>
   <si>
     <t>Evaluation</t>
+  </si>
+  <si>
+    <t>!!!!!!!!!!!!!!!!!!!!!!!!!!!!!!</t>
+  </si>
+  <si>
+    <t>(OK pour la création, faire pour la modification)</t>
+  </si>
+  <si>
+    <t>??? Voir avec le prof… la politique</t>
+  </si>
+  <si>
+    <t>Vérifier que c'est correct</t>
+  </si>
+  <si>
+    <t>A vérifier</t>
+  </si>
+  <si>
+    <t>Il n'y a pas encore les EndUsers</t>
   </si>
 </sst>
 </file>
@@ -169,7 +190,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0"/>
   </numFmts>
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -192,13 +213,45 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00B050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -214,7 +267,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -228,13 +281,52 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Pourcentage" xfId="1" builtinId="5"/>
   </cellStyles>
-  <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
+  <dxfs count="2">
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFD7D7D7"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
+  <tableStyles count="1" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4">
+    <tableStyle name="MySqlDefault" pivot="0" table="0" count="2">
+      <tableStyleElement type="wholeTable" dxfId="1"/>
+      <tableStyleElement type="headerRow" dxfId="0"/>
+    </tableStyle>
+  </tableStyles>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -562,18 +654,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E56"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A30" workbookViewId="0">
-      <selection activeCell="C56" sqref="C56"/>
+    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
+      <selection activeCell="B31" sqref="B31"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="97.83203125" customWidth="1"/>
-    <col min="4" max="4" width="19.83203125" customWidth="1"/>
+    <col min="1" max="1" width="97.875" customWidth="1"/>
+    <col min="4" max="4" width="19.875" customWidth="1"/>
     <col min="5" max="5" width="16.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="D1" s="3" t="s">
         <v>45</v>
       </c>
@@ -581,193 +673,199 @@
         <v>46</v>
       </c>
     </row>
-    <row r="2" spans="1:5">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="45">
+    <row r="3" spans="1:5" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B3">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5">
+      <c r="B3" s="7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="B4">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5">
+      <c r="B4" s="7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="B5">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5">
+      <c r="B5" s="7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="B6">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" ht="30">
+      <c r="B6" s="7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="B7">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5">
+      <c r="B7" s="7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="B8">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5">
+      <c r="B8" s="7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B9" s="3">
+      <c r="B9" s="8">
         <f>SUM(B3:B8)</f>
         <v>6</v>
       </c>
-      <c r="C9" s="4">
-        <f>B9/B$51</f>
-        <v>0.16216216216216217</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5">
+      <c r="C9" s="4"/>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="2"/>
     </row>
-    <row r="11" spans="1:5">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="12" spans="1:5">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="B12">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" ht="30">
+      <c r="B12" s="9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="B13">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" ht="30">
+      <c r="B13" s="9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="B14">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" ht="30">
+      <c r="B14" s="9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="B15">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" ht="30">
+      <c r="B15" s="9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="B16">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" ht="30">
+      <c r="B16" s="10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="B17">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3">
+      <c r="B17" s="10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="B18">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3">
+      <c r="B18" s="10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="B19">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3">
+      <c r="B19" s="10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="B20">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3">
+      <c r="B20" s="10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="B21">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3" ht="30">
+      <c r="B21" s="7">
+        <v>1</v>
+      </c>
+      <c r="C21" s="12" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A22" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="B22">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="23" spans="1:3" ht="30">
+      <c r="B22" s="10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A23" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="B23">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="24" spans="1:3" ht="30">
+      <c r="B23" s="10">
+        <v>1</v>
+      </c>
+      <c r="C23" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A24" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="B24">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="25" spans="1:3" ht="30">
+      <c r="B24" s="10">
+        <v>1</v>
+      </c>
+      <c r="C24" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A25" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="B25">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="26" spans="1:3">
+      <c r="B25" s="9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
         <v>7</v>
       </c>
@@ -780,87 +878,93 @@
         <v>0.3783783783783784</v>
       </c>
     </row>
-    <row r="27" spans="1:3">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27" s="2"/>
     </row>
-    <row r="28" spans="1:3">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="29" spans="1:3">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A29" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="B29">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="30" spans="1:3">
+      <c r="B29" s="7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A30" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="B30">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="31" spans="1:3">
+      <c r="B30" s="7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A31" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="B31">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="32" spans="1:3">
+      <c r="B31" s="9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A32" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="B32">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="33" spans="1:3">
+      <c r="B32" s="11">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A33" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="B33">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="34" spans="1:3" ht="30">
+      <c r="B33" s="11">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A34" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="B34">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="35" spans="1:3">
+      <c r="B34" s="11">
+        <v>1</v>
+      </c>
+      <c r="C34" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A35" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="B35">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="36" spans="1:3" ht="30">
+      <c r="B35" s="11">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A36" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="B36">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="37" spans="1:3">
+      <c r="B36" s="9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A37" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="B37">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="38" spans="1:3">
+      <c r="B37" s="11">
+        <v>1</v>
+      </c>
+      <c r="C37" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A38" s="1" t="s">
         <v>7</v>
       </c>
@@ -873,79 +977,82 @@
         <v>0.24324324324324326</v>
       </c>
     </row>
-    <row r="39" spans="1:3">
+    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A39" s="2"/>
     </row>
-    <row r="40" spans="1:3">
+    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A40" s="1" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="41" spans="1:3">
+    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A41" s="5" t="s">
         <v>34</v>
       </c>
-      <c r="B41">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="42" spans="1:3">
+      <c r="B41" s="11">
+        <v>1</v>
+      </c>
+      <c r="C41" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A42" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="B42">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="43" spans="1:3">
+      <c r="B42" s="11">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A43" s="5" t="s">
         <v>36</v>
       </c>
-      <c r="B43">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="44" spans="1:3" ht="30">
+      <c r="B43" s="11">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A44" s="5" t="s">
         <v>37</v>
       </c>
-      <c r="B44">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="45" spans="1:3">
+      <c r="B44" s="11">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A45" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="B45">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="46" spans="1:3" ht="30">
+      <c r="B45" s="11">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A46" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="B46">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="47" spans="1:3" ht="30">
+      <c r="B46" s="11">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A47" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="B47">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="48" spans="1:3">
+      <c r="B47" s="11">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A48" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="B48">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="49" spans="1:3">
+      <c r="B48" s="11">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A49" s="1" t="s">
         <v>7</v>
       </c>
@@ -958,10 +1065,10 @@
         <v>0.21621621621621623</v>
       </c>
     </row>
-    <row r="50" spans="1:3">
+    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A50" s="2"/>
     </row>
-    <row r="51" spans="1:3">
+    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A51" s="1" t="s">
         <v>42</v>
       </c>
@@ -970,16 +1077,16 @@
         <v>37</v>
       </c>
     </row>
-    <row r="52" spans="1:3">
+    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A52" s="2"/>
     </row>
-    <row r="53" spans="1:3">
+    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A53" s="2"/>
     </row>
-    <row r="54" spans="1:3">
+    <row r="54" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A54" s="2"/>
     </row>
-    <row r="55" spans="1:3">
+    <row r="55" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A55" s="1" t="s">
         <v>43</v>
       </c>
@@ -988,7 +1095,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="56" spans="1:3">
+    <row r="56" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A56" s="1" t="s">
         <v>44</v>
       </c>
@@ -999,6 +1106,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>

</xml_diff>

<commit_message>
Mise à jour de l'auto-evalutation
</commit_message>
<xml_diff>
--- a/evaluation/evaluation.xlsx
+++ b/evaluation/evaluation.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="52">
   <si>
     <t>LIVRABLES</t>
   </si>
@@ -166,9 +166,6 @@
   </si>
   <si>
     <t>!!!!!!!!!!!!!!!!!!!!!!!!!!!!!!</t>
-  </si>
-  <si>
-    <t>(OK pour la création, faire pour la modification)</t>
   </si>
   <si>
     <t>??? Voir avec le prof… la politique</t>
@@ -654,8 +651,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E56"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
-      <selection activeCell="B31" sqref="B31"/>
+    <sheetView tabSelected="1" topLeftCell="A18" workbookViewId="0">
+      <selection activeCell="C23" sqref="C23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -839,11 +836,8 @@
       <c r="A23" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="B23" s="10">
-        <v>1</v>
-      </c>
-      <c r="C23" t="s">
-        <v>48</v>
+      <c r="B23" s="9">
+        <v>1</v>
       </c>
     </row>
     <row r="24" spans="1:3" ht="31.5" x14ac:dyDescent="0.25">
@@ -854,7 +848,7 @@
         <v>1</v>
       </c>
       <c r="C24" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="25" spans="1:3" ht="31.5" x14ac:dyDescent="0.25">
@@ -934,7 +928,7 @@
         <v>1</v>
       </c>
       <c r="C34" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.25">
@@ -961,7 +955,7 @@
         <v>1</v>
       </c>
       <c r="C37" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.25">
@@ -993,7 +987,7 @@
         <v>1</v>
       </c>
       <c r="C41" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Mise à jour de l'auto-evaluation
</commit_message>
<xml_diff>
--- a/evaluation/evaluation.xlsx
+++ b/evaluation/evaluation.xlsx
@@ -651,8 +651,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E56"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A18" workbookViewId="0">
-      <selection activeCell="C23" sqref="C23"/>
+    <sheetView tabSelected="1" topLeftCell="A33" workbookViewId="0">
+      <selection activeCell="B37" sqref="B37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -951,7 +951,7 @@
       <c r="A37" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="B37" s="11">
+      <c r="B37" s="9">
         <v>1</v>
       </c>
       <c r="C37" t="s">

</xml_diff>

<commit_message>
Modif auto-evaluation et nombre d'utilisateurs dans les tests
</commit_message>
<xml_diff>
--- a/evaluation/evaluation.xlsx
+++ b/evaluation/evaluation.xlsx
@@ -126,18 +126,12 @@
     <t>TESTS ET VALIDATION</t>
   </si>
   <si>
-    <t>La génération des données de test a été implémentée de manière satisfaisante.</t>
-  </si>
-  <si>
     <t>Les scénarios testés par les tests d'acceptation automatisés sont décrits de manière claire dans la documentation.</t>
   </si>
   <si>
     <t>Les user acceptance tests ont été implémentés de manière satisfaisante.</t>
   </si>
   <si>
-    <t>Les objectifs et les scrénarios de tests de performance et de change sont décrits de manière claire dans la documentation.</t>
-  </si>
-  <si>
     <t>Les tests de peformance et de charge ont été implémentés de manière satisfaisante avec Jmeter.</t>
   </si>
   <si>
@@ -178,6 +172,12 @@
   </si>
   <si>
     <t>Il n'y a pas encore les EndUsers</t>
+  </si>
+  <si>
+    <t>La génération des données de test a été implémentée de manière satisfaisante (/generate)</t>
+  </si>
+  <si>
+    <t>Les objectifs et les scrénarios de tests de performance et de charge sont décrits de manière claire dans la documentation. (Jmeter)</t>
   </si>
 </sst>
 </file>
@@ -219,7 +219,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -250,6 +250,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -264,7 +270,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -284,6 +290,9 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="49" fontId="0" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -651,8 +660,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E56"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A33" workbookViewId="0">
-      <selection activeCell="B37" sqref="B37"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="A16" sqref="A16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -664,10 +673,10 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="D1" s="3" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="E1" s="3" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
@@ -821,7 +830,7 @@
         <v>1</v>
       </c>
       <c r="C21" s="12" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
     </row>
     <row r="22" spans="1:3" ht="31.5" x14ac:dyDescent="0.25">
@@ -848,7 +857,7 @@
         <v>1</v>
       </c>
       <c r="C24" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
     </row>
     <row r="25" spans="1:3" ht="31.5" x14ac:dyDescent="0.25">
@@ -928,7 +937,7 @@
         <v>1</v>
       </c>
       <c r="C34" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.25">
@@ -955,7 +964,7 @@
         <v>1</v>
       </c>
       <c r="C37" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.25">
@@ -981,18 +990,18 @@
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A41" s="5" t="s">
-        <v>34</v>
+        <v>50</v>
       </c>
       <c r="B41" s="11">
         <v>1</v>
       </c>
       <c r="C41" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A42" s="5" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B42" s="11">
         <v>1</v>
@@ -1000,7 +1009,7 @@
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A43" s="5" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B43" s="11">
         <v>1</v>
@@ -1008,7 +1017,7 @@
     </row>
     <row r="44" spans="1:3" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A44" s="5" t="s">
-        <v>37</v>
+        <v>51</v>
       </c>
       <c r="B44" s="11">
         <v>1</v>
@@ -1016,7 +1025,7 @@
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A45" s="2" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="B45" s="11">
         <v>1</v>
@@ -1024,15 +1033,15 @@
     </row>
     <row r="46" spans="1:3" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A46" s="2" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="B46" s="11">
         <v>1</v>
       </c>
     </row>
     <row r="47" spans="1:3" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A47" s="2" t="s">
-        <v>40</v>
+      <c r="A47" s="13" t="s">
+        <v>38</v>
       </c>
       <c r="B47" s="11">
         <v>1</v>
@@ -1040,7 +1049,7 @@
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A48" s="2" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="B48" s="11">
         <v>1</v>
@@ -1064,7 +1073,7 @@
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A51" s="1" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="B51" s="3">
         <f>SUM(B9,B26,B38,B49)</f>
@@ -1082,7 +1091,7 @@
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A55" s="1" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="B55" s="3">
         <f>B51-B48-B26</f>
@@ -1091,7 +1100,7 @@
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A56" s="1" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="B56" s="6">
         <f>B55/B51*5+1</f>

</xml_diff>

<commit_message>
Mise à jour auto-evalutation
</commit_message>
<xml_diff>
--- a/evaluation/evaluation.xlsx
+++ b/evaluation/evaluation.xlsx
@@ -168,9 +168,6 @@
     <t>Vérifier que c'est correct</t>
   </si>
   <si>
-    <t>A vérifier</t>
-  </si>
-  <si>
     <t>Il n'y a pas encore les EndUsers</t>
   </si>
   <si>
@@ -178,6 +175,9 @@
   </si>
   <si>
     <t>Les objectifs et les scrénarios de tests de performance et de charge sont décrits de manière claire dans la documentation. (Jmeter)</t>
+  </si>
+  <si>
+    <t>OK car le répertoire WEB-INF est protégé !</t>
   </si>
 </sst>
 </file>
@@ -660,8 +660,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E56"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="A16" sqref="A16"/>
+    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
+      <selection activeCell="A36" sqref="A36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -964,7 +964,7 @@
         <v>1</v>
       </c>
       <c r="C37" t="s">
-        <v>48</v>
+        <v>51</v>
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.25">
@@ -990,13 +990,13 @@
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A41" s="5" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B41" s="11">
         <v>1</v>
       </c>
       <c r="C41" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.25">
@@ -1017,7 +1017,7 @@
     </row>
     <row r="44" spans="1:3" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A44" s="5" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B44" s="11">
         <v>1</v>

</xml_diff>

<commit_message>
Mise à jour de l'auto-évaluation
</commit_message>
<xml_diff>
--- a/evaluation/evaluation.xlsx
+++ b/evaluation/evaluation.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="54">
   <si>
     <t>LIVRABLES</t>
   </si>
@@ -165,9 +165,6 @@
     <t>??? Voir avec le prof… la politique</t>
   </si>
   <si>
-    <t>Vérifier que c'est correct</t>
-  </si>
-  <si>
     <t>Il n'y a pas encore les EndUsers</t>
   </si>
   <si>
@@ -178,6 +175,15 @@
   </si>
   <si>
     <t>OK car le répertoire WEB-INF est protégé !</t>
+  </si>
+  <si>
+    <t>Presque bon</t>
+  </si>
+  <si>
+    <t>A faire par Vanessa</t>
+  </si>
+  <si>
+    <t>A FAIRE !!</t>
   </si>
 </sst>
 </file>
@@ -660,8 +666,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E56"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
-      <selection activeCell="A36" sqref="A36"/>
+    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="B41" sqref="B41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -789,12 +795,15 @@
       <c r="B16" s="10">
         <v>1</v>
       </c>
+      <c r="C16" t="s">
+        <v>52</v>
+      </c>
     </row>
     <row r="17" spans="1:3" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="B17" s="10">
+      <c r="B17" s="9">
         <v>1</v>
       </c>
     </row>
@@ -805,12 +814,15 @@
       <c r="B18" s="10">
         <v>1</v>
       </c>
+      <c r="C18" t="s">
+        <v>51</v>
+      </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="B19" s="10">
+      <c r="B19" s="9">
         <v>1</v>
       </c>
     </row>
@@ -821,6 +833,9 @@
       <c r="B20" s="10">
         <v>1</v>
       </c>
+      <c r="C20" t="s">
+        <v>51</v>
+      </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" s="2" t="s">
@@ -920,6 +935,9 @@
       <c r="B32" s="11">
         <v>1</v>
       </c>
+      <c r="C32" s="3" t="s">
+        <v>53</v>
+      </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A33" s="2" t="s">
@@ -928,23 +946,23 @@
       <c r="B33" s="11">
         <v>1</v>
       </c>
+      <c r="C33" s="3" t="s">
+        <v>53</v>
+      </c>
     </row>
     <row r="34" spans="1:3" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A34" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="B34" s="11">
-        <v>1</v>
-      </c>
-      <c r="C34" t="s">
-        <v>47</v>
+      <c r="B34" s="9">
+        <v>1</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A35" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="B35" s="11">
+      <c r="B35" s="9">
         <v>1</v>
       </c>
     </row>
@@ -964,7 +982,7 @@
         <v>1</v>
       </c>
       <c r="C37" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.25">
@@ -990,13 +1008,13 @@
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A41" s="5" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B41" s="11">
         <v>1</v>
       </c>
       <c r="C41" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.25">
@@ -1017,7 +1035,7 @@
     </row>
     <row r="44" spans="1:3" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A44" s="5" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B44" s="11">
         <v>1</v>

</xml_diff>

<commit_message>
Mise à jour evaluation
</commit_message>
<xml_diff>
--- a/evaluation/evaluation.xlsx
+++ b/evaluation/evaluation.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="53">
   <si>
     <t>LIVRABLES</t>
   </si>
@@ -177,13 +177,10 @@
     <t>OK car le répertoire WEB-INF est protégé !</t>
   </si>
   <si>
-    <t>Presque bon</t>
-  </si>
-  <si>
-    <t>A faire par Vanessa</t>
-  </si>
-  <si>
     <t>A FAIRE !!</t>
+  </si>
+  <si>
+    <t>Reste : Style pour la page courante</t>
   </si>
 </sst>
 </file>
@@ -666,8 +663,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E56"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="B41" sqref="B41"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -811,11 +808,8 @@
       <c r="A18" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="B18" s="10">
-        <v>1</v>
-      </c>
-      <c r="C18" t="s">
-        <v>51</v>
+      <c r="B18" s="9">
+        <v>1</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
@@ -833,9 +827,6 @@
       <c r="B20" s="10">
         <v>1</v>
       </c>
-      <c r="C20" t="s">
-        <v>51</v>
-      </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" s="2" t="s">
@@ -852,7 +843,7 @@
       <c r="A22" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="B22" s="10">
+      <c r="B22" s="9">
         <v>1</v>
       </c>
     </row>
@@ -936,7 +927,7 @@
         <v>1</v>
       </c>
       <c r="C32" s="3" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.25">
@@ -947,7 +938,7 @@
         <v>1</v>
       </c>
       <c r="C33" s="3" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
     </row>
     <row r="34" spans="1:3" ht="31.5" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Mise à jour du rapport et de l'évaluation
</commit_message>
<xml_diff>
--- a/evaluation/evaluation.xlsx
+++ b/evaluation/evaluation.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="52">
   <si>
     <t>LIVRABLES</t>
   </si>
@@ -157,9 +157,6 @@
   </si>
   <si>
     <t>Evaluation</t>
-  </si>
-  <si>
-    <t>!!!!!!!!!!!!!!!!!!!!!!!!!!!!!!</t>
   </si>
   <si>
     <t>??? Voir avec le prof… la politique</t>
@@ -663,8 +660,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E56"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="B16" sqref="B16"/>
+    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
+      <selection activeCell="A45" sqref="A45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -793,7 +790,7 @@
         <v>1</v>
       </c>
       <c r="C16" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="17" spans="1:3" ht="31.5" x14ac:dyDescent="0.25">
@@ -824,7 +821,7 @@
       <c r="A20" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="B20" s="10">
+      <c r="B20" s="9">
         <v>1</v>
       </c>
     </row>
@@ -832,12 +829,10 @@
       <c r="A21" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="B21" s="7">
-        <v>1</v>
-      </c>
-      <c r="C21" s="12" t="s">
-        <v>45</v>
-      </c>
+      <c r="B21" s="9">
+        <v>1</v>
+      </c>
+      <c r="C21" s="12"/>
     </row>
     <row r="22" spans="1:3" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A22" s="2" t="s">
@@ -863,7 +858,7 @@
         <v>1</v>
       </c>
       <c r="C24" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="25" spans="1:3" ht="31.5" x14ac:dyDescent="0.25">
@@ -927,7 +922,7 @@
         <v>1</v>
       </c>
       <c r="C32" s="3" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.25">
@@ -938,7 +933,7 @@
         <v>1</v>
       </c>
       <c r="C33" s="3" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="34" spans="1:3" ht="31.5" x14ac:dyDescent="0.25">
@@ -973,7 +968,7 @@
         <v>1</v>
       </c>
       <c r="C37" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.25">
@@ -999,13 +994,13 @@
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A41" s="5" t="s">
-        <v>48</v>
-      </c>
-      <c r="B41" s="11">
+        <v>47</v>
+      </c>
+      <c r="B41" s="9">
         <v>1</v>
       </c>
       <c r="C41" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.25">
@@ -1026,7 +1021,7 @@
     </row>
     <row r="44" spans="1:3" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A44" s="5" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B44" s="11">
         <v>1</v>

</xml_diff>

<commit_message>
Ajout de l'attribut title dans les controleurs pour les titres des pages
</commit_message>
<xml_diff>
--- a/evaluation/evaluation.xlsx
+++ b/evaluation/evaluation.xlsx
@@ -1,8 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Henri\Desktop\HEIG-SEM5\AMT\Projet\Teaching-HEIGVD-AMT-2015-Project\evaluation\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="240" yWindow="240" windowWidth="20730" windowHeight="11760" tabRatio="500"/>
   </bookViews>
@@ -12,7 +17,7 @@
   <definedNames>
     <definedName name="LOCAL_MYSQL_DATE_FORMAT" hidden="1">REPT(LOCAL_YEAR_FORMAT,4)&amp;LOCAL_DATE_SEPARATOR&amp;REPT(LOCAL_MONTH_FORMAT,2)&amp;LOCAL_DATE_SEPARATOR&amp;REPT(LOCAL_DAY_FORMAT,2)&amp;" "&amp;REPT(LOCAL_HOUR_FORMAT,2)&amp;LOCAL_TIME_SEPARATOR&amp;REPT(LOCAL_MINUTE_FORMAT,2)&amp;LOCAL_TIME_SEPARATOR&amp;REPT(LOCAL_SECOND_FORMAT,2)</definedName>
   </definedNames>
-  <calcPr calcId="145621" concurrentCalc="0"/>
+  <calcPr calcId="152511" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -331,6 +336,9 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -660,8 +668,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E56"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
-      <selection activeCell="A45" sqref="A45"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A36" sqref="A36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
JSP création et modification account factorisé
</commit_message>
<xml_diff>
--- a/evaluation/evaluation.xlsx
+++ b/evaluation/evaluation.xlsx
@@ -1,13 +1,8 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Henri\Desktop\HEIG-SEM5\AMT\Projet\Teaching-HEIGVD-AMT-2015-Project\evaluation\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="240" yWindow="240" windowWidth="20730" windowHeight="11760" tabRatio="500"/>
   </bookViews>
@@ -27,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="52">
   <si>
     <t>LIVRABLES</t>
   </si>
@@ -668,8 +663,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E56"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A36" sqref="A36"/>
+    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
+      <selection activeCell="C33" sqref="C33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -937,12 +932,10 @@
       <c r="A33" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="B33" s="11">
-        <v>1</v>
-      </c>
-      <c r="C33" s="3" t="s">
-        <v>50</v>
-      </c>
+      <c r="B33" s="9">
+        <v>1</v>
+      </c>
+      <c r="C33" s="3"/>
     </row>
     <row r="34" spans="1:3" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A34" s="2" t="s">

</xml_diff>

<commit_message>
Mise à jour du rapport et de l'auto-évaluation
</commit_message>
<xml_diff>
--- a/evaluation/evaluation.xlsx
+++ b/evaluation/evaluation.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="54">
   <si>
     <t>LIVRABLES</t>
   </si>
@@ -178,9 +178,6 @@
   </si>
   <si>
     <t>vanessa</t>
-  </si>
-  <si>
-    <t>Raphaël</t>
   </si>
   <si>
     <t>Raphaël : Contrôleur, Services (non DAO)   /   Alex :  Entités JPA, DTO, Services DAO</t>
@@ -679,8 +676,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E56"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="A29" sqref="A29"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="C24" sqref="C24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -879,11 +876,8 @@
       <c r="A24" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="B24" s="10">
-        <v>1</v>
-      </c>
-      <c r="C24" t="s">
-        <v>52</v>
+      <c r="B24" s="9">
+        <v>1</v>
       </c>
     </row>
     <row r="25" spans="1:3" ht="31.5" x14ac:dyDescent="0.25">
@@ -923,7 +917,7 @@
         <v>1</v>
       </c>
       <c r="C29" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.25">
@@ -934,7 +928,7 @@
         <v>1</v>
       </c>
       <c r="C30" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Adding test and write part of report
</commit_message>
<xml_diff>
--- a/evaluation/evaluation.xlsx
+++ b/evaluation/evaluation.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="5" rupBuild="4507"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="240" windowWidth="20730" windowHeight="11760" tabRatio="500"/>
@@ -189,11 +189,11 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0"/>
   </numFmts>
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="5">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -282,7 +282,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -306,10 +306,11 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Pourcentage" xfId="1" builtinId="5"/>
+    <cellStyle name="Percent" xfId="1" builtinId="5"/>
   </cellStyles>
   <dxfs count="2">
     <dxf>
@@ -673,21 +674,21 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:E56"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C29" sqref="C29:C30"/>
+    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
+      <selection activeCell="B46" sqref="B46"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
   <cols>
     <col min="1" max="1" width="97.875" customWidth="1"/>
     <col min="4" max="4" width="19.875" customWidth="1"/>
     <col min="5" max="5" width="16.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5">
       <c r="D1" s="3" t="s">
         <v>43</v>
       </c>
@@ -695,12 +696,12 @@
         <v>44</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="47.25" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" ht="47.25">
       <c r="A3" s="2" t="s">
         <v>1</v>
       </c>
@@ -711,7 +712,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5">
       <c r="A4" s="2" t="s">
         <v>2</v>
       </c>
@@ -719,7 +720,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5">
       <c r="A5" s="2" t="s">
         <v>3</v>
       </c>
@@ -727,7 +728,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5">
       <c r="A6" s="2" t="s">
         <v>4</v>
       </c>
@@ -738,7 +739,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="7" spans="1:5" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" ht="31.5">
       <c r="A7" s="2" t="s">
         <v>5</v>
       </c>
@@ -749,7 +750,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5">
       <c r="A8" s="2" t="s">
         <v>6</v>
       </c>
@@ -757,7 +758,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5">
       <c r="A9" s="1" t="s">
         <v>7</v>
       </c>
@@ -767,15 +768,15 @@
       </c>
       <c r="C9" s="4"/>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5">
       <c r="A10" s="2"/>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5">
       <c r="A11" s="1" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5">
       <c r="A12" s="2" t="s">
         <v>9</v>
       </c>
@@ -783,7 +784,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:5" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5" ht="31.5">
       <c r="A13" s="2" t="s">
         <v>10</v>
       </c>
@@ -791,7 +792,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:5" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:5" ht="31.5">
       <c r="A14" s="2" t="s">
         <v>11</v>
       </c>
@@ -799,7 +800,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:5" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:5" ht="31.5">
       <c r="A15" s="2" t="s">
         <v>12</v>
       </c>
@@ -807,7 +808,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:5" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:5" ht="31.5">
       <c r="A16" s="2" t="s">
         <v>13</v>
       </c>
@@ -818,7 +819,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="17" spans="1:3" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:3" ht="31.5">
       <c r="A17" s="2" t="s">
         <v>14</v>
       </c>
@@ -826,7 +827,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:3">
       <c r="A18" s="2" t="s">
         <v>15</v>
       </c>
@@ -834,7 +835,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:3">
       <c r="A19" s="2" t="s">
         <v>16</v>
       </c>
@@ -842,7 +843,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:3">
       <c r="A20" s="2" t="s">
         <v>17</v>
       </c>
@@ -850,7 +851,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:3">
       <c r="A21" s="2" t="s">
         <v>18</v>
       </c>
@@ -859,7 +860,7 @@
       </c>
       <c r="C21" s="12"/>
     </row>
-    <row r="22" spans="1:3" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:3" ht="31.5">
       <c r="A22" s="2" t="s">
         <v>19</v>
       </c>
@@ -867,7 +868,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="23" spans="1:3" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:3" ht="31.5">
       <c r="A23" s="2" t="s">
         <v>20</v>
       </c>
@@ -875,7 +876,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="24" spans="1:3" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:3" ht="31.5">
       <c r="A24" s="2" t="s">
         <v>21</v>
       </c>
@@ -883,7 +884,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="25" spans="1:3" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:3" ht="31.5">
       <c r="A25" s="2" t="s">
         <v>22</v>
       </c>
@@ -891,7 +892,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:3">
       <c r="A26" s="1" t="s">
         <v>7</v>
       </c>
@@ -904,15 +905,15 @@
         <v>0.3783783783783784</v>
       </c>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:3">
       <c r="A27" s="2"/>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:3">
       <c r="A28" s="1" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:3">
       <c r="A29" s="2" t="s">
         <v>24</v>
       </c>
@@ -920,7 +921,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:3">
       <c r="A30" s="2" t="s">
         <v>25</v>
       </c>
@@ -928,7 +929,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:3">
       <c r="A31" s="2" t="s">
         <v>26</v>
       </c>
@@ -936,7 +937,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:3">
       <c r="A32" s="2" t="s">
         <v>27</v>
       </c>
@@ -945,7 +946,7 @@
       </c>
       <c r="C32" s="3"/>
     </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:3">
       <c r="A33" s="2" t="s">
         <v>28</v>
       </c>
@@ -954,7 +955,7 @@
       </c>
       <c r="C33" s="3"/>
     </row>
-    <row r="34" spans="1:3" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:3" ht="31.5">
       <c r="A34" s="2" t="s">
         <v>29</v>
       </c>
@@ -962,7 +963,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:3">
       <c r="A35" s="2" t="s">
         <v>30</v>
       </c>
@@ -970,7 +971,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="36" spans="1:3" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:3" ht="31.5">
       <c r="A36" s="2" t="s">
         <v>31</v>
       </c>
@@ -978,7 +979,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:3">
       <c r="A37" s="2" t="s">
         <v>32</v>
       </c>
@@ -989,7 +990,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:3">
       <c r="A38" s="1" t="s">
         <v>7</v>
       </c>
@@ -1002,15 +1003,15 @@
         <v>0.24324324324324326</v>
       </c>
     </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:3">
       <c r="A39" s="2"/>
     </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:3">
       <c r="A40" s="1" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:3">
       <c r="A41" s="5" t="s">
         <v>46</v>
       </c>
@@ -1021,7 +1022,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:3">
       <c r="A42" s="5" t="s">
         <v>34</v>
       </c>
@@ -1032,40 +1033,40 @@
         <v>53</v>
       </c>
     </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:3">
       <c r="A43" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="B43" s="11">
+      <c r="B43" s="9">
         <v>1</v>
       </c>
       <c r="C43" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="44" spans="1:3" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:3" ht="31.5">
       <c r="A44" s="5" t="s">
         <v>47</v>
       </c>
-      <c r="B44" s="11">
+      <c r="B44" s="15">
         <v>1</v>
       </c>
       <c r="C44" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:3">
       <c r="A45" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="B45" s="11">
+      <c r="B45" s="9">
         <v>1</v>
       </c>
       <c r="C45" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="46" spans="1:3" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:3" ht="31.5">
       <c r="A46" s="2" t="s">
         <v>37</v>
       </c>
@@ -1076,7 +1077,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="47" spans="1:3" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:3" ht="31.5">
       <c r="A47" s="13" t="s">
         <v>38</v>
       </c>
@@ -1087,15 +1088,15 @@
         <v>53</v>
       </c>
     </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:3">
       <c r="A48" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="B48" s="11">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B48" s="9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3">
       <c r="A49" s="1" t="s">
         <v>7</v>
       </c>
@@ -1108,10 +1109,10 @@
         <v>0.21621621621621623</v>
       </c>
     </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:3">
       <c r="A50" s="2"/>
     </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:3">
       <c r="A51" s="1" t="s">
         <v>40</v>
       </c>
@@ -1120,16 +1121,16 @@
         <v>37</v>
       </c>
     </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:3">
       <c r="A52" s="2"/>
     </row>
-    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:3">
       <c r="A53" s="2"/>
     </row>
-    <row r="54" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:3">
       <c r="A54" s="2"/>
     </row>
-    <row r="55" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:3">
       <c r="A55" s="1" t="s">
         <v>41</v>
       </c>
@@ -1138,7 +1139,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="56" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:3">
       <c r="A56" s="1" t="s">
         <v>42</v>
       </c>

</xml_diff>

<commit_message>
Avancement de ma partie du rapport
</commit_message>
<xml_diff>
--- a/evaluation/evaluation.xlsx
+++ b/evaluation/evaluation.xlsx
@@ -677,7 +677,7 @@
   <dimension ref="A1:E56"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C16" sqref="C16"/>
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -704,7 +704,7 @@
       <c r="A3" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="7">
+      <c r="B3" s="9">
         <v>1</v>
       </c>
       <c r="C3" t="s">
@@ -742,7 +742,7 @@
       <c r="A7" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="B7" s="7">
+      <c r="B7" s="9">
         <v>1</v>
       </c>
       <c r="C7" t="s">

</xml_diff>